<commit_message>
DONE: New parsing line TODO: improve offset computing algo
</commit_message>
<xml_diff>
--- a/RTE_Configurator test plan.xlsx
+++ b/RTE_Configurator test plan.xlsx
@@ -560,9 +560,6 @@
     <t xml:space="preserve">Check that the order is respected when dealing with SWC-MODE-SWITCH-EVENT </t>
   </si>
   <si>
-    <t>Check that the tool will manage an existing cycke between different tasks</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -615,67 +612,12 @@
     <t>YES</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">- check if the corresponding error is present in the log
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- check that the output script is not created</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">- check if the corresponding error is present in the log (event 2 has an EVENTS-CALLED and is referenced in another EVENTS-CALLED)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- check that the output script is not created</t>
-    </r>
-  </si>
-  <si>
     <t>RTECONFIG.1</t>
   </si>
   <si>
     <t>RTECONFIG.2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- check that the output arxml file is not produced</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-- check the log for the corresponding error</t>
-    </r>
-  </si>
-  <si>
     <t>- check that the DATA-RECEIVED-EVENT is present in the script, and its RteMappedToTaskRef parameter has the correct form: TaskApp_CORE_PARTITION_EVT</t>
   </si>
   <si>
@@ -1008,20 +950,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Test 9: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provide to the tool two arxml files where each one contains one event (event1  and event2), one swc allocation file where for both events, COREs and PARTITIONs are the same and one event constraint file where  &lt;CONTAIN-IMPLICIT-ACCESS&gt; attribute is set to 'false', &lt;UNMAPPED&gt; attribute is set to '1" and event1 has an EVENTS-CALLED to event2</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -1114,39 +1042,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>EVENTS-CALLED not set, and one swc allocation file where for both events, COREs and PARTITIONs are different.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Test 8: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Provide to the tool two arxml files where each one contains one event(event1  and event2), one swc allocation file where for both events, COREs and PARTITIONs are the same and one event constraint file where  &lt;CONTAIN-IMPLICIT-ACCESS&gt; attribute is set to 'false', &lt;UNMAPPED&gt; attribute is set to "true" and event1 has an EVENTS-CALLED</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to event2</t>
     </r>
   </si>
   <si>
@@ -1228,13 +1123,81 @@
   </si>
   <si>
     <t>RTE.EXCEPT.OIE</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test 9: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provide to the tool two arxml files where each one contains one OIE event (event1  and event2), one swc allocation file where for both events, COREs and PARTITIONs are the same and one event constraint file where  &lt;CONTAIN-IMPLICIT-ACCESS&gt; attribute is set to 'false', &lt;UNMAPPED&gt; attribute is set to '1" and event1 has an EVENTS-CALLED to event2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Test 8: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Provide to the tool two arxml files where each one contains one OIE event(event1  and event2), one swc allocation file where for both events, COREs and PARTITIONs are the same and one event constraint file where  &lt;CONTAIN-IMPLICIT-ACCESS&gt; attribute is set to 'false', &lt;UNMAPPED&gt; attribute is set to "true" and event1 has an EVENTS-CALLED</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to event2</t>
+    </r>
+  </si>
+  <si>
+    <t>Check that the tool will manage an existing cycle between different tasks</t>
+  </si>
+  <si>
+    <t>- check if the corresponding error is present in the log</t>
+  </si>
+  <si>
+    <t>- check if the corresponding error is present in the log (event 2 has an EVENTS-CALLED and is referenced in another EVENTS-CALLED)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- check the log for the corresponding error</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1246,13 +1209,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1686,31 +1642,31 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1719,20 +1675,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1744,6 +1700,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1753,82 +1721,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2302,16 +2208,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" style="45" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38" style="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="79.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" style="1" customWidth="1"/>
@@ -2353,10 +2259,10 @@
         <v>4</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2373,15 +2279,15 @@
         <v>28</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="49" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>31</v>
@@ -2393,10 +2299,10 @@
         <v>32</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2404,26 +2310,26 @@
         <v>33</v>
       </c>
       <c r="B5" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>72</v>
-      </c>
       <c r="D5" s="25" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="58" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="59" t="s">
+      <c r="A6" s="60" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="61" t="s">
         <v>41</v>
       </c>
       <c r="C6" s="18" t="s">
@@ -2433,62 +2339,62 @@
         <v>43</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="58"/>
-      <c r="B7" s="59"/>
+      <c r="A7" s="60"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="18" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="58"/>
-      <c r="B8" s="59"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="18" t="s">
         <v>45</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="59"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="18" t="s">
         <v>46</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>76</v>
+        <v>120</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
         <v>47</v>
       </c>
@@ -2496,16 +2402,16 @@
         <v>48</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>77</v>
+        <v>121</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2522,15 +2428,15 @@
         <v>52</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>53</v>
@@ -2542,101 +2448,101 @@
         <v>55</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="59" t="s">
+      <c r="A13" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="61" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="58"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D14" s="48" t="s">
         <v>56</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="47" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D15" s="48" t="s">
         <v>56</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="58"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="47" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D16" s="48" t="s">
         <v>57</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="58"/>
-      <c r="B17" s="59"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="47" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>57</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="52" t="s">
-        <v>93</v>
-      </c>
-      <c r="B18" s="55" t="s">
+      <c r="A18" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="52" t="s">
         <v>58</v>
       </c>
       <c r="C18" s="18" t="s">
@@ -2646,47 +2552,47 @@
         <v>60</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="56"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="59"/>
       <c r="C19" s="18" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="53"/>
-      <c r="B20" s="56"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="37" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D20" s="25" t="s">
         <v>60</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="53"/>
-      <c r="B21" s="56"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="18" t="s">
         <v>61</v>
       </c>
@@ -2694,65 +2600,65 @@
         <v>60</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="53"/>
-      <c r="B22" s="56"/>
+      <c r="A22" s="57"/>
+      <c r="B22" s="59"/>
       <c r="C22" s="18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D22" s="25" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="53"/>
-      <c r="B23" s="56"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="59"/>
       <c r="C23" s="18" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A24" s="54"/>
-      <c r="B24" s="57"/>
+      <c r="A24" s="58"/>
+      <c r="B24" s="53"/>
       <c r="C24" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D24" s="25" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="B25" s="59" t="s">
+      <c r="A25" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" s="61" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -2762,15 +2668,15 @@
         <v>37</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="18" t="s">
         <v>38</v>
       </c>
@@ -2778,15 +2684,15 @@
         <v>35</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="58"/>
-      <c r="B27" s="59"/>
+      <c r="A27" s="60"/>
+      <c r="B27" s="61"/>
       <c r="C27" s="18" t="s">
         <v>40</v>
       </c>
@@ -2794,15 +2700,15 @@
         <v>39</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B28" s="28" t="s">
         <v>62</v>
@@ -2814,10 +2720,10 @@
         <v>63</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -2834,10 +2740,10 @@
         <v>68</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2848,169 +2754,169 @@
         <v>70</v>
       </c>
       <c r="C30" s="37" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D30" s="25" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="B31" s="55" t="s">
-        <v>96</v>
+      <c r="A31" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="52" t="s">
+        <v>92</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
-      <c r="B32" s="56"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="59"/>
       <c r="C32" s="46" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D32" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
-      <c r="B33" s="56"/>
+      <c r="A33" s="57"/>
+      <c r="B33" s="59"/>
       <c r="C33" s="46" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D33" s="25" t="s">
         <v>56</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="57"/>
+      <c r="B34" s="59"/>
       <c r="C34" s="46" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D34" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
-      <c r="B35" s="56"/>
+      <c r="A35" s="57"/>
+      <c r="B35" s="59"/>
       <c r="C35" s="46" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D35" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="53"/>
-      <c r="B36" s="56"/>
+      <c r="A36" s="57"/>
+      <c r="B36" s="59"/>
       <c r="C36" s="46" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D36" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="53"/>
-      <c r="B37" s="56"/>
+      <c r="A37" s="57"/>
+      <c r="B37" s="59"/>
       <c r="C37" s="46" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D37" s="25" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="53"/>
-      <c r="B38" s="56"/>
+      <c r="A38" s="57"/>
+      <c r="B38" s="59"/>
       <c r="C38" s="46" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D38" s="25" t="s">
         <v>57</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="54"/>
-      <c r="B39" s="57"/>
+      <c r="A39" s="58"/>
+      <c r="B39" s="53"/>
       <c r="C39" s="46" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>57</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="42" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B40" s="29" t="s">
         <v>19</v>
@@ -3019,63 +2925,63 @@
         <v>20</v>
       </c>
       <c r="D40" s="25" t="s">
-        <v>80</v>
+        <v>122</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" s="55" t="s">
-        <v>118</v>
+      <c r="A41" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>112</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D41" s="25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="61"/>
-      <c r="B42" s="57"/>
+      <c r="A42" s="55"/>
+      <c r="B42" s="53"/>
       <c r="C42" s="21" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D42" s="25" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="43" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B43" s="38" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D43" s="40" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E43" s="35" t="s">
         <v>11</v>
@@ -3086,7 +2992,7 @@
     </row>
     <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B44" s="32" t="s">
         <v>21</v>
@@ -3106,43 +3012,43 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E29"/>
   <mergeCells count="12">
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="A18:A24"/>
     <mergeCell ref="B41:B42"/>
     <mergeCell ref="A41:A42"/>
     <mergeCell ref="A31:A39"/>
     <mergeCell ref="B31:B39"/>
     <mergeCell ref="A25:A27"/>
     <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="A18:A24"/>
   </mergeCells>
   <conditionalFormatting sqref="E48:E1048576 E1:E45">
-    <cfRule type="cellIs" dxfId="9" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="19" operator="equal">
       <formula>"done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
       <formula>"not done"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F44">
-    <cfRule type="cellIs" dxfId="7" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
       <formula>"N/A"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F44">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>